<commit_message>
div changes and add ons
</commit_message>
<xml_diff>
--- a/faktura_generator/faktura_mal.xlsx
+++ b/faktura_generator/faktura_mal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\Fakturagenerator\faktura_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19864F8D-A5A8-4A1F-8E9E-79AD26B55306}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5541E8AE-53E3-407F-A6BC-78EA2D4063E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5422331E-21C7-414D-85E7-2AEDA28BF89C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5422331E-21C7-414D-85E7-2AEDA28BF89C}"/>
   </bookViews>
   <sheets>
     <sheet name="4" sheetId="5" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Beskrivelse</t>
   </si>
@@ -257,18 +257,22 @@
   </si>
   <si>
     <t>Totalt</t>
+  </si>
+  <si>
+    <t>Totalt_antall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-&quot;kr&quot;\ * #,##0.00_-;\-&quot;kr&quot;\ * #,##0.00_-;_-&quot;kr&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0_ ;\-0\ "/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="_-[$kr-414]\ * #,##0.00_-;\-[$kr-414]\ * #,##0.00_-;_-[$kr-414]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="&quot;kr&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -515,7 +519,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -838,25 +842,25 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="8.36328125" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" customWidth="1"/>
-    <col min="15" max="15" width="12.90625" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -893,13 +897,17 @@
       <c r="L1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>52</v>
+      <c r="B2" t="str">
+        <f>IF(A2=1, "Anette Evensen", "N/A")</f>
+        <v>Anette Evensen</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -918,6 +926,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="27">
+        <f>F2*G2</f>
         <v>0</v>
       </c>
       <c r="I2" s="27">
@@ -931,11 +940,15 @@
         <v>63</v>
       </c>
       <c r="L2" s="30">
-        <f>SUM(I2:I3)</f>
+        <f>SUM(F2:F3)</f>
         <v>495</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M2" s="4">
+        <f>SUM(C2:C3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -959,20 +972,27 @@
         <v>0</v>
       </c>
       <c r="H3" s="27">
+        <f>F3*G3</f>
         <v>0</v>
       </c>
       <c r="I3" s="27">
-        <f>SUM(I2)</f>
+        <f>F3+H3</f>
         <v>247.5</v>
       </c>
       <c r="J3" s="1">
-        <v>43941</v>
+        <v>43937</v>
       </c>
       <c r="K3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
       <c r="D4" s="27"/>
       <c r="E4" s="4"/>
       <c r="F4" s="26"/>
@@ -980,14 +1000,17 @@
       <c r="H4" s="27"/>
       <c r="I4" s="27"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="D5" s="27"/>
       <c r="E5" s="4"/>
       <c r="F5" s="26"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6" s="27"/>
       <c r="F6" s="26"/>
       <c r="G6" s="25"/>
@@ -997,7 +1020,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" s="27"/>
       <c r="G7" s="25"/>
       <c r="H7" s="27"/>
@@ -1006,7 +1029,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" s="27"/>
       <c r="G8" s="25"/>
       <c r="H8" s="27"/>
@@ -1015,7 +1038,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
       <c r="D9" s="27"/>
       <c r="E9" s="4"/>
@@ -1027,7 +1050,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
       <c r="D10" s="27"/>
       <c r="E10" s="4"/>
@@ -1038,7 +1061,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="F11" s="7"/>
@@ -1047,29 +1070,29 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1091,17 +1114,17 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="43.26953125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="31.7265625" style="8" customWidth="1"/>
-    <col min="4" max="5" width="15.54296875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="2.7265625" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="8"/>
+    <col min="1" max="1" width="2.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="8" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="24" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:5" s="24" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="29" t="s">
         <v>51</v>
       </c>
@@ -1109,7 +1132,7 @@
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
     </row>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
         <v>50</v>
       </c>
@@ -1117,7 +1140,7 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
     </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22">
         <v>2020</v>
       </c>
@@ -1125,18 +1148,18 @@
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>47</v>
       </c>
@@ -1144,7 +1167,7 @@
         <v>34500</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>46</v>
       </c>
@@ -1152,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>45</v>
       </c>
@@ -1161,46 +1184,46 @@
         <v>34500</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="16"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="14"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="14"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="14"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>38</v>
       </c>
@@ -1209,13 +1232,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="18"/>
     </row>
-    <row r="18" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
@@ -1224,10 +1247,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>35</v>
       </c>
@@ -1236,76 +1259,76 @@
         <v>34500</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="14"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="14"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="14"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D29" s="14"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="14"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="14"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="14"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="12" t="s">
         <v>23</v>
       </c>
@@ -1314,37 +1337,37 @@
         <v>1705.56</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="14"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="14"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="14"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="14"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="14"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="12" t="s">
         <v>17</v>
       </c>
@@ -1352,31 +1375,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="14"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="14"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="14"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="14"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="12" t="s">
         <v>12</v>
       </c>
@@ -1384,7 +1407,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="12" t="s">
         <v>11</v>
       </c>
@@ -1393,25 +1416,25 @@
         <v>5544</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="14"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="14"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D48" s="14"/>
     </row>
-    <row r="49" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>7</v>
       </c>
@@ -1420,10 +1443,10 @@
         <v>7847.5599999999995</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="11"/>
     </row>
-    <row r="51" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="11" t="s">
         <v>6</v>
       </c>
@@ -1432,27 +1455,27 @@
         <v>26652.440000000002</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="12"/>
     </row>
-    <row r="53" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D54" s="14"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D55" s="14"/>
     </row>
-    <row r="56" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="s">
         <v>2</v>
       </c>
@@ -1461,10 +1484,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="12"/>
     </row>
-    <row r="58" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>1</v>
       </c>
@@ -1473,10 +1496,10 @@
         <v>26652.440000000002</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B59" s="9"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="9"/>
     </row>
   </sheetData>

</xml_diff>